<commit_message>
added optimized compression aware bipartite
Still need to figure out why normal bipartite isn't as efficient as compression aware one
</commit_message>
<xml_diff>
--- a/Algorithm_results.xlsx
+++ b/Algorithm_results.xlsx
@@ -415,11 +415,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1553226304"/>
-        <c:axId val="1542648944"/>
+        <c:axId val="-131907952"/>
+        <c:axId val="-144295520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1553226304"/>
+        <c:axId val="-131907952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,12 +531,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542648944"/>
+        <c:crossAx val="-144295520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1542648944"/>
+        <c:axId val="-144295520"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -654,7 +654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1553226304"/>
+        <c:crossAx val="-131907952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1099,11 +1099,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1542677392"/>
-        <c:axId val="1542681152"/>
+        <c:axId val="-132450944"/>
+        <c:axId val="-132448512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1542677392"/>
+        <c:axId val="-132450944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,12 +1215,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542681152"/>
+        <c:crossAx val="-132448512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1542681152"/>
+        <c:axId val="-132448512"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1333,7 +1333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542677392"/>
+        <c:crossAx val="-132450944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1459,7 +1459,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1687,11 +1686,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1542713296"/>
-        <c:axId val="1501150432"/>
+        <c:axId val="-132417504"/>
+        <c:axId val="-132413744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1542713296"/>
+        <c:axId val="-132417504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1736,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1803,12 +1801,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1501150432"/>
+        <c:crossAx val="-132413744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1501150432"/>
+        <c:axId val="-132413744"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1855,7 +1853,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1921,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542713296"/>
+        <c:crossAx val="-132417504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1935,7 +1932,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2047,7 +2043,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2367,11 +2362,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1542724496"/>
-        <c:axId val="1542728256"/>
+        <c:axId val="-98257920"/>
+        <c:axId val="-99026512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1542724496"/>
+        <c:axId val="-98257920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2417,7 +2412,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2483,12 +2477,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542728256"/>
+        <c:crossAx val="-99026512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1542728256"/>
+        <c:axId val="-99026512"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2535,7 +2529,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2601,7 +2594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542724496"/>
+        <c:crossAx val="-98257920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2615,7 +2608,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6606,8 +6598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N78" sqref="N78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>